<commit_message>
back to campus commit
</commit_message>
<xml_diff>
--- a/SPRING 20/CSE 101 Non CSE/Section 4/online_attendance_cse101_sec4.xlsx
+++ b/SPRING 20/CSE 101 Non CSE/Section 4/online_attendance_cse101_sec4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\SPRING 20\CSE 101 Non CSE\Section 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E83DBB-C574-4F74-B331-E7909E667AB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A04479-8BA9-4A65-B013-56B647533887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>SL</t>
   </si>
@@ -181,6 +181,30 @@
   </si>
   <si>
     <t>p</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>Mid Marks</t>
+  </si>
+  <si>
+    <t>Convert to</t>
+  </si>
+  <si>
+    <t>Mid Total</t>
+  </si>
+  <si>
+    <t>Mid Impact</t>
+  </si>
+  <si>
+    <t>Mid Impact Raw</t>
+  </si>
+  <si>
+    <t>Free Marks</t>
+  </si>
+  <si>
+    <t>Attendance</t>
   </si>
 </sst>
 </file>
@@ -273,7 +297,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -686,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -699,10 +743,12 @@
     <col min="3" max="3" width="30.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" style="8" customWidth="1"/>
     <col min="5" max="5" width="10" style="7"/>
-    <col min="6" max="16384" width="10" style="1"/>
+    <col min="6" max="7" width="10" style="1"/>
+    <col min="8" max="15" width="15.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -715,8 +761,23 @@
       <c r="D1" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -727,8 +788,30 @@
         <v>3</v>
       </c>
       <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>181011267</v>
+      </c>
+      <c r="G2" s="1">
+        <f>IF(D2="p",3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <f>(H2/$E$55)*$E$56</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>ROUND(I2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <f>G2+J2+$E$57</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -739,8 +822,30 @@
         <v>4</v>
       </c>
       <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>182014067</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G47" si="0">IF(D3="p",3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I47" si="1">(H3/$E$55)*$E$56</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J47" si="2">ROUND(I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K47" si="3">G3+J3+$E$57</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -751,8 +856,30 @@
         <v>5</v>
       </c>
       <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>183013067</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -765,8 +892,30 @@
       <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>191011047</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -777,8 +926,30 @@
         <v>7</v>
       </c>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>191013041</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -791,8 +962,30 @@
       <c r="D7" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <v>192011082</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -803,8 +996,30 @@
         <v>9</v>
       </c>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <v>192011115</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -815,8 +1030,30 @@
         <v>10</v>
       </c>
       <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <v>193011146</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -827,8 +1064,30 @@
         <v>11</v>
       </c>
       <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <v>193012057</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -841,8 +1100,30 @@
       <c r="D11" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <v>193013072</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>20</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -855,8 +1136,30 @@
       <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <v>193013094</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>16</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -867,8 +1170,30 @@
         <v>14</v>
       </c>
       <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <v>201011087</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -879,8 +1204,30 @@
         <v>15</v>
       </c>
       <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <v>201011091</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -893,8 +1240,30 @@
       <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <v>201011130</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>22</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -907,8 +1276,30 @@
       <c r="D16" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <v>201011131</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H16" s="1">
+        <v>21</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -921,8 +1312,30 @@
       <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <v>201011143</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -933,8 +1346,30 @@
         <v>19</v>
       </c>
       <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <v>201011146</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -947,8 +1382,30 @@
       <c r="D19" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <v>201011199</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H19" s="1">
+        <v>20</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -959,8 +1416,30 @@
         <v>21</v>
       </c>
       <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <v>201011212</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>17</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -973,8 +1452,30 @@
       <c r="D21" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <v>201012032</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H21" s="1">
+        <v>19</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -985,8 +1486,30 @@
         <v>23</v>
       </c>
       <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <v>201012055</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>19</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -999,8 +1522,30 @@
       <c r="D23" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <v>201012063</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H23" s="1">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -1011,8 +1556,30 @@
         <v>25</v>
       </c>
       <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <v>201012079</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>24</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -1025,8 +1592,30 @@
       <c r="D25" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="1">
+        <v>201013012</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H25" s="1">
+        <v>19</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1039,8 +1628,30 @@
       <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="1">
+        <v>201013028</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H26" s="1">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K26" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -1051,8 +1662,30 @@
         <v>28</v>
       </c>
       <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="1">
+        <v>201013030</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -1063,8 +1696,30 @@
         <v>29</v>
       </c>
       <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="1">
+        <v>201013032</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>20</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -1075,8 +1730,30 @@
         <v>30</v>
       </c>
       <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="1">
+        <v>201013033</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>17</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="1"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -1089,8 +1766,30 @@
       <c r="D30" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="1">
+        <v>201013036</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H30" s="1">
+        <v>21</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -1101,8 +1800,30 @@
         <v>32</v>
       </c>
       <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="1">
+        <v>201013039</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>12</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -1115,8 +1836,30 @@
       <c r="D32" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="1">
+        <v>201013046</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H32" s="1">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -1129,8 +1872,30 @@
       <c r="D33" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="1">
+        <v>201013053</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H33" s="1">
+        <v>22</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -1143,8 +1908,30 @@
       <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F34" s="1">
+        <v>201013063</v>
+      </c>
+      <c r="G34" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>24</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -1157,8 +1944,30 @@
       <c r="D35" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="1">
+        <v>201013074</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>22</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -1169,8 +1978,30 @@
         <v>37</v>
       </c>
       <c r="D36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="1">
+        <v>201013075</v>
+      </c>
+      <c r="G36" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>21</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -1183,8 +2014,30 @@
       <c r="D37" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="1">
+        <v>201013076</v>
+      </c>
+      <c r="G37" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>22</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
@@ -1197,8 +2050,30 @@
       <c r="D38" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="1">
+        <v>201013081</v>
+      </c>
+      <c r="G38" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>20</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J38" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>38</v>
       </c>
@@ -1209,8 +2084,30 @@
         <v>40</v>
       </c>
       <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F39" s="1">
+        <v>201013087</v>
+      </c>
+      <c r="G39" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>20</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -1223,8 +2120,30 @@
       <c r="D40" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>201013090</v>
+      </c>
+      <c r="G40" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H40" s="1">
+        <v>23</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="1"/>
+        <v>9.2000000000000011</v>
+      </c>
+      <c r="J40" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -1235,8 +2154,30 @@
         <v>42</v>
       </c>
       <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F41" s="1">
+        <v>201013100</v>
+      </c>
+      <c r="G41" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>21</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -1249,8 +2190,30 @@
       <c r="D42" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F42" s="1">
+        <v>201013102</v>
+      </c>
+      <c r="G42" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H42" s="1">
+        <v>21</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="1"/>
+        <v>8.4</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -1261,8 +2224,30 @@
         <v>44</v>
       </c>
       <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="1">
+        <v>201013104</v>
+      </c>
+      <c r="G43" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>20</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J43" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -1275,8 +2260,30 @@
       <c r="D44" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F44" s="1">
+        <v>201013110</v>
+      </c>
+      <c r="G44" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H44" s="1">
+        <v>20</v>
+      </c>
+      <c r="I44" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J44" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>44</v>
       </c>
@@ -1289,8 +2296,30 @@
       <c r="D45" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F45" s="1">
+        <v>201013114</v>
+      </c>
+      <c r="G45" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>20</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>45</v>
       </c>
@@ -1303,8 +2332,30 @@
       <c r="D46" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F46" s="1">
+        <v>201014075</v>
+      </c>
+      <c r="G46" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H46" s="1">
+        <v>20</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J46" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -1317,29 +2368,82 @@
       <c r="D47" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="1">
+        <v>201016013</v>
+      </c>
+      <c r="G47" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H47" s="1">
+        <v>20</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J47" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="K47" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="8">
         <f>COUNTIF(D2:D47,"=p")</f>
         <v>25</v>
       </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F51" s="4"/>
+    </row>
+    <row r="55" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E56" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="7">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:XFD47">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$E2 &gt; 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F47">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>$B$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>